<commit_message>
Add filter, aggr and projsel
</commit_message>
<xml_diff>
--- a/cust_transactions.xlsx
+++ b/cust_transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\Redis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmpat\Documents\DMST\Redis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4DBBF3-9F73-4A25-920B-8976D4A544FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB648F9-B1F5-4355-B02D-CCCA34831FE5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{78478C0E-7084-466D-A739-149D7398006B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{78478C0E-7084-466D-A739-149D7398006B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,39 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Customer ID</t>
   </si>
   <si>
     <t>Transaction ID</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>t8</t>
-  </si>
-  <si>
-    <t>t9</t>
-  </si>
-  <si>
-    <t>t3</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>t7</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
-    <t>t1</t>
   </si>
 </sst>
 </file>
@@ -104,7 +77,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -120,7 +93,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,19 +389,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A23B826-A3B0-40E7-B9F0-271064A82881}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,236 +409,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>7098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>2867</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>3667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>8759</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>8677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>1116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>